<commit_message>
Scripting SCD0226 - Sales melakukan Simulasi Performance Calculator and Re-run SCD0195 - Pimpinan Wilayah Mengakses Menu Report - Menu Product Holding Ratio - Report
</commit_message>
<xml_diff>
--- a/Lib_Repo_Excel/FileExcel_Digisales/SCD0195 - Pimpinan Wilayah Mengakses Menu Report - Menu Product Holding Ratio - Report.xlsx
+++ b/Lib_Repo_Excel/FileExcel_Digisales/SCD0195 - Pimpinan Wilayah Mengakses Menu Report - Menu Product Holding Ratio - Report.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\1442\Desktop\DigiSales\Lib_Repo_Excel\FileExcel_Digisales\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\1427\Documents\BNI\DigiSales\Lib_Repo_Excel\FileExcel_Digisales\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CF8DB7B-DC50-4ADE-846B-6AD936CE8029}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{031301B7-A959-460C-9C48-A51B01AEB9E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2640" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SCD0195" sheetId="2" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
   <si>
     <t>SIDEBAR_MENU</t>
   </si>
@@ -74,67 +74,22 @@
     <t>TEXT2</t>
   </si>
   <si>
-    <t>FILE1</t>
-  </si>
-  <si>
     <t>Product Holding</t>
   </si>
   <si>
     <t>TEXT3</t>
   </si>
   <si>
-    <t>ReportProductHolding.xlsx</t>
-  </si>
-  <si>
     <t>TEXT4</t>
   </si>
   <si>
     <t>TEXT5</t>
   </si>
   <si>
-    <t>QUERY1</t>
-  </si>
-  <si>
-    <t>QUERY2</t>
-  </si>
-  <si>
-    <t>QUERY3</t>
-  </si>
-  <si>
-    <t>EXPL_QUERY1</t>
-  </si>
-  <si>
-    <t>EXPL_QUERY2</t>
-  </si>
-  <si>
-    <t>EXPL_QUERY3</t>
-  </si>
-  <si>
-    <t>USER_DB</t>
-  </si>
-  <si>
-    <t>PASSWORD_DB</t>
-  </si>
-  <si>
-    <t>HOSTNAME</t>
-  </si>
-  <si>
-    <t>sa</t>
-  </si>
-  <si>
-    <t>4eFfEJAA!</t>
-  </si>
-  <si>
-    <t>192.168.232.6</t>
-  </si>
-  <si>
     <t>Pimpinan Wilayah mengakses menu: Report Menu - Product Holding Ratio - Report</t>
   </si>
   <si>
     <t>Pimpinan Wilayah</t>
-  </si>
-  <si>
-    <t>SELECT * FROM DigisalesNew..Tbl_Pegawai as p JOIN DigisalesNew..Tbl_Unit as u on p.Unit_Id = u.Id JOIN DigisalesNew..Tbl_Unit_Wilayah as uw on u.wilayah_id = uw.id where u.wilayah_id = '12' and role_id = '4' order by p.nama</t>
   </si>
   <si>
     <t>1. login digisales portal dengan pimpinan wilayah 18994
@@ -207,7 +162,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -233,9 +188,20 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -545,8 +511,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0EAF5E5-8229-45B3-AC11-8AED029F52F4}">
   <dimension ref="A1:Z6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -575,143 +541,116 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="N1" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="O1" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q1" s="9"/>
+      <c r="R1" s="9"/>
+      <c r="S1" s="9"/>
+      <c r="T1" s="9"/>
+      <c r="U1" s="9"/>
+      <c r="V1" s="9"/>
+      <c r="W1" s="9"/>
+      <c r="X1" s="9"/>
+      <c r="Y1" s="9"/>
+      <c r="Z1" s="9"/>
+    </row>
+    <row r="2" spans="1:26" ht="102" x14ac:dyDescent="0.25">
+      <c r="A2" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="D2" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="F2" s="11">
+        <v>18994</v>
+      </c>
+      <c r="G2" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="I2" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="R1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="U1" s="1" t="s">
+      <c r="J2" s="12"/>
+      <c r="K2" s="12"/>
+      <c r="L2" s="12">
+        <v>39798</v>
+      </c>
+      <c r="M2" s="12">
+        <v>2022</v>
+      </c>
+      <c r="N2" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="V1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="X1" t="s">
-        <v>26</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>27</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="2" spans="1:26" ht="240" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="C2" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="F2" s="3">
-        <v>18994</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="L2" s="1">
-        <v>39798</v>
-      </c>
-      <c r="M2" s="1">
-        <v>2022</v>
-      </c>
-      <c r="N2" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="O2" s="5"/>
-      <c r="P2" s="5"/>
-      <c r="Q2" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="R2" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="U2" s="10" t="str">
-        <f>"Pembuktian Sales yang ada pada User " &amp; F2</f>
-        <v>Pembuktian Sales yang ada pada User 18994</v>
-      </c>
-      <c r="X2" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="Y2" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="Z2" s="10" t="s">
-        <v>31</v>
-      </c>
+      <c r="O2" s="13"/>
+      <c r="P2" s="13"/>
+      <c r="Q2" s="13"/>
+      <c r="R2" s="12"/>
+      <c r="S2" s="12"/>
+      <c r="T2" s="12"/>
+      <c r="U2" s="12"/>
+      <c r="V2" s="12"/>
+      <c r="W2" s="12"/>
+      <c r="X2" s="11"/>
+      <c r="Y2" s="11"/>
+      <c r="Z2" s="12"/>
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B3" s="6"/>

</xml_diff>